<commit_message>
automatic denoising using user specified options
</commit_message>
<xml_diff>
--- a/Results-Generation/subj0/results_Alpha.xlsx
+++ b/Results-Generation/subj0/results_Alpha.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Layers Number</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>Noise</t>
+  </si>
+  <si>
+    <t>eyescrunching</t>
+  </si>
+  <si>
+    <t>jaw</t>
+  </si>
+  <si>
+    <t>raisingeyebrows</t>
+  </si>
+  <si>
+    <t>movehat</t>
+  </si>
+  <si>
+    <t>movehead</t>
   </si>
 </sst>
 </file>
@@ -434,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,6 +520,331 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2.5</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>15</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0.01</v>
+      </c>
+      <c r="P2">
+        <v>0.01</v>
+      </c>
+      <c r="Q2">
+        <v>-0.03954538461277818</v>
+      </c>
+      <c r="R2">
+        <v>26.62025762178805</v>
+      </c>
+      <c r="S2">
+        <v>16.31018336053107</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2.5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.01</v>
+      </c>
+      <c r="P3">
+        <v>0.01</v>
+      </c>
+      <c r="Q3">
+        <v>-0.02081399515663128</v>
+      </c>
+      <c r="R3">
+        <v>23.06462261758369</v>
+      </c>
+      <c r="S3">
+        <v>21.83555164121976</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2.5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.01</v>
+      </c>
+      <c r="P4">
+        <v>0.01</v>
+      </c>
+      <c r="Q4">
+        <v>-0.03782867504932325</v>
+      </c>
+      <c r="R4">
+        <v>16.43695554907289</v>
+      </c>
+      <c r="S4">
+        <v>-14.5564680488108</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2.5</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0.001</v>
+      </c>
+      <c r="P5">
+        <v>0.001</v>
+      </c>
+      <c r="Q5">
+        <v>-3.04077830408176</v>
+      </c>
+      <c r="R5">
+        <v>9.925443034519448</v>
+      </c>
+      <c r="S5">
+        <v>-4.67507000742246</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2.5</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.01</v>
+      </c>
+      <c r="P6">
+        <v>0.1</v>
+      </c>
+      <c r="Q6">
+        <v>-0.03688754513089874</v>
+      </c>
+      <c r="R6">
+        <v>1.56427737596919</v>
+      </c>
+      <c r="S6">
+        <v>-8.457205793158687</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added t test to autmation
</commit_message>
<xml_diff>
--- a/Results-Generation/subj0/results_Alpha.xlsx
+++ b/Results-Generation/subj0/results_Alpha.xlsx
@@ -573,7 +573,7 @@
         <v>-0.03954538461277818</v>
       </c>
       <c r="R2">
-        <v>26.62025762178805</v>
+        <v>26.12878482475952</v>
       </c>
       <c r="S2">
         <v>16.31018336053107</v>
@@ -638,7 +638,7 @@
         <v>-0.02081399515663128</v>
       </c>
       <c r="R3">
-        <v>23.06462261758369</v>
+        <v>24.78110472640491</v>
       </c>
       <c r="S3">
         <v>21.83555164121976</v>

</xml_diff>

<commit_message>
updated automation of the whole DNF system
</commit_message>
<xml_diff>
--- a/Results-Generation/subj0/results_Alpha.xlsx
+++ b/Results-Generation/subj0/results_Alpha.xlsx
@@ -573,7 +573,7 @@
         <v>-0.03954538461277818</v>
       </c>
       <c r="R2">
-        <v>26.12878482475952</v>
+        <v>28.44618809978375</v>
       </c>
       <c r="S2">
         <v>16.31018336053107</v>
@@ -638,7 +638,7 @@
         <v>-0.02081399515663128</v>
       </c>
       <c r="R3">
-        <v>24.78110472640491</v>
+        <v>26.0805135663567</v>
       </c>
       <c r="S3">
         <v>21.83555164121976</v>
@@ -703,10 +703,10 @@
         <v>-0.03782867504932325</v>
       </c>
       <c r="R4">
-        <v>16.43695554907289</v>
+        <v>28.08518718029109</v>
       </c>
       <c r="S4">
-        <v>-14.5564680488108</v>
+        <v>18.76295454903327</v>
       </c>
       <c r="T4">
         <v>2</v>
@@ -768,10 +768,10 @@
         <v>-3.04077830408176</v>
       </c>
       <c r="R5">
-        <v>9.925443034519448</v>
+        <v>1.553820082092557</v>
       </c>
       <c r="S5">
-        <v>-4.67507000742246</v>
+        <v>-0.4416577113042988</v>
       </c>
       <c r="T5">
         <v>3</v>
@@ -833,10 +833,10 @@
         <v>-0.03688754513089874</v>
       </c>
       <c r="R6">
-        <v>1.56427737596919</v>
+        <v>25.64080623124418</v>
       </c>
       <c r="S6">
-        <v>-8.457205793158687</v>
+        <v>-9.408754405736811</v>
       </c>
       <c r="T6">
         <v>4</v>

</xml_diff>